<commit_message>
brightness_analysys_1a - add graph
</commit_message>
<xml_diff>
--- a/sov_extract/Data/brightness_analys_5_26_01.xlsx
+++ b/sov_extract/Data/brightness_analys_5_26_01.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N65"/>
+  <dimension ref="A1:O65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,19 +447,20 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="4" customWidth="1" min="1" max="1"/>
-    <col width="11" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
     <col width="8" customWidth="1" min="4" max="4"/>
     <col width="10" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="7" customWidth="1" min="7" max="7"/>
-    <col width="11" customWidth="1" min="8" max="8"/>
-    <col width="7" customWidth="1" min="9" max="9"/>
-    <col width="12" customWidth="1" min="10" max="10"/>
-    <col width="7" customWidth="1" min="11" max="11"/>
-    <col width="11" customWidth="1" min="12" max="12"/>
-    <col width="7" customWidth="1" min="13" max="13"/>
-    <col width="12" customWidth="1" min="14" max="14"/>
+    <col width="6" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="7" customWidth="1" min="8" max="8"/>
+    <col width="11" customWidth="1" min="9" max="9"/>
+    <col width="7" customWidth="1" min="10" max="10"/>
+    <col width="12" customWidth="1" min="11" max="11"/>
+    <col width="7" customWidth="1" min="12" max="12"/>
+    <col width="11" customWidth="1" min="13" max="13"/>
+    <col width="7" customWidth="1" min="14" max="14"/>
+    <col width="12" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -485,45 +486,50 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>used pixels %</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>L20</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>us_pixL20</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>U235</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>us_pixU235</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>L40</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>us_pixL40</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>U215</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>us_pixU215</t>
         </is>
@@ -533,10 +539,8 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>a_01k.png</t>
-        </is>
+      <c r="B2" t="n">
+        <v>1</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -552,41 +556,42 @@
         <v>147.8</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" t="n">
         <v>147.8</v>
       </c>
-      <c r="H2" t="n">
-        <v>1</v>
-      </c>
       <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="n">
         <v>147.8</v>
       </c>
-      <c r="J2" t="n">
-        <v>1</v>
-      </c>
       <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
         <v>147.9</v>
       </c>
-      <c r="L2" t="n">
-        <v>1</v>
-      </c>
       <c r="M2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" t="n">
         <v>147.9</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>a_01s.png</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -595,48 +600,49 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Sm</t>
+          <t>Kam</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>203.8</v>
+        <v>148.7</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G3" t="n">
-        <v>203.5</v>
+        <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>1</v>
+        <v>147.8</v>
       </c>
       <c r="I3" t="n">
-        <v>203.5</v>
+        <v>1</v>
       </c>
       <c r="J3" t="n">
-        <v>1</v>
+        <v>147.8</v>
       </c>
       <c r="K3" t="n">
-        <v>192.2</v>
+        <v>1</v>
       </c>
       <c r="L3" t="n">
-        <v>0.6</v>
+        <v>148.7</v>
       </c>
       <c r="M3" t="n">
-        <v>192.2</v>
+        <v>1</v>
       </c>
       <c r="N3" t="n">
-        <v>0.6</v>
+        <v>148.7</v>
+      </c>
+      <c r="O3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>a_02k.png</t>
-        </is>
+        <v>8</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -649,44 +655,45 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>148.7</v>
+        <v>154.4</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G4" t="n">
-        <v>147.8</v>
+        <v>1</v>
       </c>
       <c r="H4" t="n">
-        <v>1</v>
+        <v>154.4</v>
       </c>
       <c r="I4" t="n">
-        <v>147.8</v>
+        <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>1</v>
+        <v>154.4</v>
       </c>
       <c r="K4" t="n">
-        <v>148.7</v>
+        <v>1</v>
       </c>
       <c r="L4" t="n">
-        <v>1</v>
+        <v>154.4</v>
       </c>
       <c r="M4" t="n">
-        <v>148.7</v>
+        <v>1</v>
       </c>
       <c r="N4" t="n">
+        <v>154.4</v>
+      </c>
+      <c r="O4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>a_02s.png</t>
-        </is>
+        <v>12</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -695,48 +702,49 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Sm</t>
+          <t>Kam</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>202.5</v>
+        <v>148.6</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="G5" t="n">
-        <v>200.5</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>1</v>
+        <v>148.6</v>
       </c>
       <c r="I5" t="n">
-        <v>200.5</v>
+        <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>1</v>
+        <v>148.6</v>
       </c>
       <c r="K5" t="n">
-        <v>186.4</v>
+        <v>1</v>
       </c>
       <c r="L5" t="n">
-        <v>0.5</v>
+        <v>148.6</v>
       </c>
       <c r="M5" t="n">
-        <v>186.4</v>
+        <v>1</v>
       </c>
       <c r="N5" t="n">
-        <v>0.5</v>
+        <v>148.6</v>
+      </c>
+      <c r="O5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>a_03k.png</t>
-        </is>
+        <v>16</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -749,44 +757,45 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>154.4</v>
+        <v>154.5</v>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G6" t="n">
-        <v>154.4</v>
+        <v>1</v>
       </c>
       <c r="H6" t="n">
-        <v>1</v>
+        <v>154.5</v>
       </c>
       <c r="I6" t="n">
-        <v>154.4</v>
+        <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>1</v>
+        <v>154.5</v>
       </c>
       <c r="K6" t="n">
-        <v>154.4</v>
+        <v>1</v>
       </c>
       <c r="L6" t="n">
-        <v>1</v>
+        <v>154.5</v>
       </c>
       <c r="M6" t="n">
-        <v>154.4</v>
+        <v>1</v>
       </c>
       <c r="N6" t="n">
+        <v>154.5</v>
+      </c>
+      <c r="O6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>a_03s.png</t>
-        </is>
+        <v>20</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -795,48 +804,49 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Sm</t>
+          <t>Kam</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>207</v>
+        <v>159.8</v>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G7" t="n">
-        <v>206.9</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>1</v>
+        <v>159.8</v>
       </c>
       <c r="I7" t="n">
-        <v>206.9</v>
+        <v>1</v>
       </c>
       <c r="J7" t="n">
-        <v>1</v>
+        <v>159.8</v>
       </c>
       <c r="K7" t="n">
-        <v>194.9</v>
+        <v>1</v>
       </c>
       <c r="L7" t="n">
-        <v>0.5</v>
+        <v>159.8</v>
       </c>
       <c r="M7" t="n">
-        <v>194.9</v>
+        <v>1</v>
       </c>
       <c r="N7" t="n">
-        <v>0.5</v>
+        <v>159.8</v>
+      </c>
+      <c r="O7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>a_04k.png</t>
-        </is>
+        <v>24</v>
+      </c>
+      <c r="B8" t="n">
+        <v>7</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -849,44 +859,45 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>148.6</v>
+        <v>156.5</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G8" t="n">
-        <v>148.6</v>
+        <v>1</v>
       </c>
       <c r="H8" t="n">
-        <v>1</v>
+        <v>156</v>
       </c>
       <c r="I8" t="n">
-        <v>148.6</v>
+        <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>1</v>
+        <v>156</v>
       </c>
       <c r="K8" t="n">
-        <v>148.6</v>
+        <v>1</v>
       </c>
       <c r="L8" t="n">
-        <v>1</v>
+        <v>156.5</v>
       </c>
       <c r="M8" t="n">
-        <v>148.6</v>
+        <v>1</v>
       </c>
       <c r="N8" t="n">
+        <v>156.5</v>
+      </c>
+      <c r="O8" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>a_04s.png</t>
-        </is>
+        <v>28</v>
+      </c>
+      <c r="B9" t="n">
+        <v>8</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -895,48 +906,49 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Sm</t>
+          <t>Kam</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>196.4</v>
+        <v>161.4</v>
       </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G9" t="n">
-        <v>196.1</v>
+        <v>1</v>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>161.4</v>
       </c>
       <c r="I9" t="n">
-        <v>196.1</v>
+        <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>1</v>
+        <v>161.4</v>
       </c>
       <c r="K9" t="n">
-        <v>176.6</v>
+        <v>1</v>
       </c>
       <c r="L9" t="n">
-        <v>0.6</v>
+        <v>161.4</v>
       </c>
       <c r="M9" t="n">
-        <v>176.6</v>
+        <v>1</v>
       </c>
       <c r="N9" t="n">
-        <v>0.6</v>
+        <v>161.4</v>
+      </c>
+      <c r="O9" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>a_05k.png</t>
-        </is>
+        <v>32</v>
+      </c>
+      <c r="B10" t="n">
+        <v>9</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -949,44 +961,45 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>154.5</v>
+        <v>163.7</v>
       </c>
       <c r="F10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10" t="n">
-        <v>154.5</v>
+        <v>1</v>
       </c>
       <c r="H10" t="n">
-        <v>1</v>
+        <v>163.7</v>
       </c>
       <c r="I10" t="n">
-        <v>154.5</v>
+        <v>1</v>
       </c>
       <c r="J10" t="n">
-        <v>1</v>
+        <v>163.7</v>
       </c>
       <c r="K10" t="n">
-        <v>154.5</v>
+        <v>1</v>
       </c>
       <c r="L10" t="n">
-        <v>1</v>
+        <v>163.7</v>
       </c>
       <c r="M10" t="n">
-        <v>154.5</v>
+        <v>1</v>
       </c>
       <c r="N10" t="n">
+        <v>163.7</v>
+      </c>
+      <c r="O10" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>a_05s.png</t>
-        </is>
+        <v>36</v>
+      </c>
+      <c r="B11" t="n">
+        <v>10</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -995,48 +1008,49 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Sm</t>
+          <t>Kam</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>208.3</v>
+        <v>164.8</v>
       </c>
       <c r="F11" t="n">
         <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>208.1</v>
+        <v>1</v>
       </c>
       <c r="H11" t="n">
-        <v>1</v>
+        <v>164.8</v>
       </c>
       <c r="I11" t="n">
-        <v>208.1</v>
+        <v>1</v>
       </c>
       <c r="J11" t="n">
-        <v>1</v>
+        <v>164.8</v>
       </c>
       <c r="K11" t="n">
-        <v>190.9</v>
+        <v>1</v>
       </c>
       <c r="L11" t="n">
-        <v>0.4</v>
+        <v>164.8</v>
       </c>
       <c r="M11" t="n">
-        <v>190.9</v>
+        <v>1</v>
       </c>
       <c r="N11" t="n">
-        <v>0.4</v>
+        <v>164.8</v>
+      </c>
+      <c r="O11" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>a_06k.png</t>
-        </is>
+        <v>40</v>
+      </c>
+      <c r="B12" t="n">
+        <v>11</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -1049,44 +1063,45 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>159.8</v>
+        <v>163.1</v>
       </c>
       <c r="F12" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G12" t="n">
-        <v>159.8</v>
+        <v>1</v>
       </c>
       <c r="H12" t="n">
-        <v>1</v>
+        <v>163.1</v>
       </c>
       <c r="I12" t="n">
-        <v>159.8</v>
+        <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>1</v>
+        <v>163.1</v>
       </c>
       <c r="K12" t="n">
-        <v>159.8</v>
+        <v>1</v>
       </c>
       <c r="L12" t="n">
-        <v>1</v>
+        <v>163.1</v>
       </c>
       <c r="M12" t="n">
-        <v>159.8</v>
+        <v>1</v>
       </c>
       <c r="N12" t="n">
+        <v>163.1</v>
+      </c>
+      <c r="O12" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>a_06s.png</t>
-        </is>
+        <v>44</v>
+      </c>
+      <c r="B13" t="n">
+        <v>12</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -1095,48 +1110,49 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Sm</t>
+          <t>Kam</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>211.3</v>
+        <v>158.4</v>
       </c>
       <c r="F13" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G13" t="n">
-        <v>211.1</v>
+        <v>1</v>
       </c>
       <c r="H13" t="n">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c r="I13" t="n">
-        <v>211.1</v>
+        <v>1</v>
       </c>
       <c r="J13" t="n">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c r="K13" t="n">
-        <v>182.1</v>
+        <v>1</v>
       </c>
       <c r="L13" t="n">
-        <v>0.3</v>
+        <v>158.4</v>
       </c>
       <c r="M13" t="n">
-        <v>182.1</v>
+        <v>1</v>
       </c>
       <c r="N13" t="n">
-        <v>0.3</v>
+        <v>158.4</v>
+      </c>
+      <c r="O13" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>a_07k.png</t>
-        </is>
+        <v>48</v>
+      </c>
+      <c r="B14" t="n">
+        <v>13</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -1149,44 +1165,45 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>156.5</v>
+        <v>155.6</v>
       </c>
       <c r="F14" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G14" t="n">
-        <v>156</v>
+        <v>1</v>
       </c>
       <c r="H14" t="n">
-        <v>1</v>
+        <v>155.4</v>
       </c>
       <c r="I14" t="n">
-        <v>156</v>
+        <v>1</v>
       </c>
       <c r="J14" t="n">
-        <v>1</v>
+        <v>155.4</v>
       </c>
       <c r="K14" t="n">
-        <v>156.5</v>
+        <v>1</v>
       </c>
       <c r="L14" t="n">
-        <v>1</v>
+        <v>155.6</v>
       </c>
       <c r="M14" t="n">
-        <v>156.5</v>
+        <v>1</v>
       </c>
       <c r="N14" t="n">
+        <v>155.6</v>
+      </c>
+      <c r="O14" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>a_07s.png</t>
-        </is>
+        <v>52</v>
+      </c>
+      <c r="B15" t="n">
+        <v>14</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -1195,48 +1212,49 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Sm</t>
+          <t>Kam</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>208.7</v>
+        <v>161.1</v>
       </c>
       <c r="F15" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G15" t="n">
-        <v>207.2</v>
+        <v>1</v>
       </c>
       <c r="H15" t="n">
-        <v>1</v>
+        <v>161.1</v>
       </c>
       <c r="I15" t="n">
-        <v>207.2</v>
+        <v>1</v>
       </c>
       <c r="J15" t="n">
-        <v>1</v>
+        <v>161.1</v>
       </c>
       <c r="K15" t="n">
-        <v>159.8</v>
+        <v>1</v>
       </c>
       <c r="L15" t="n">
-        <v>0.2</v>
+        <v>161.1</v>
       </c>
       <c r="M15" t="n">
-        <v>159.8</v>
+        <v>1</v>
       </c>
       <c r="N15" t="n">
-        <v>0.2</v>
+        <v>161.1</v>
+      </c>
+      <c r="O15" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>a_08k.png</t>
-        </is>
+        <v>56</v>
+      </c>
+      <c r="B16" t="n">
+        <v>15</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -1249,44 +1267,45 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>161.4</v>
+        <v>163.7</v>
       </c>
       <c r="F16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G16" t="n">
-        <v>161.4</v>
+        <v>1</v>
       </c>
       <c r="H16" t="n">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="I16" t="n">
-        <v>161.4</v>
+        <v>1</v>
       </c>
       <c r="J16" t="n">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="K16" t="n">
-        <v>161.4</v>
+        <v>1</v>
       </c>
       <c r="L16" t="n">
-        <v>1</v>
+        <v>163.7</v>
       </c>
       <c r="M16" t="n">
-        <v>161.4</v>
+        <v>1</v>
       </c>
       <c r="N16" t="n">
+        <v>163.7</v>
+      </c>
+      <c r="O16" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>a_08s.png</t>
-        </is>
+        <v>60</v>
+      </c>
+      <c r="B17" t="n">
+        <v>16</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -1295,48 +1314,49 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Sm</t>
+          <t>Kam</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>213.5</v>
+        <v>158.2</v>
       </c>
       <c r="F17" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G17" t="n">
-        <v>213</v>
+        <v>1</v>
       </c>
       <c r="H17" t="n">
-        <v>1</v>
+        <v>157.9</v>
       </c>
       <c r="I17" t="n">
-        <v>213</v>
+        <v>1</v>
       </c>
       <c r="J17" t="n">
-        <v>1</v>
+        <v>157.9</v>
       </c>
       <c r="K17" t="n">
-        <v>159.8</v>
+        <v>1</v>
       </c>
       <c r="L17" t="n">
-        <v>0.2</v>
+        <v>158.2</v>
       </c>
       <c r="M17" t="n">
-        <v>159.8</v>
+        <v>1</v>
       </c>
       <c r="N17" t="n">
-        <v>0.2</v>
+        <v>158.2</v>
+      </c>
+      <c r="O17" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>a_09k.png</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -1345,48 +1365,49 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Kam</t>
+          <t>Sm</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>163.7</v>
+        <v>203.8</v>
       </c>
       <c r="F18" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G18" t="n">
-        <v>163.7</v>
+        <v>1</v>
       </c>
       <c r="H18" t="n">
-        <v>1</v>
+        <v>203.5</v>
       </c>
       <c r="I18" t="n">
-        <v>163.7</v>
+        <v>1</v>
       </c>
       <c r="J18" t="n">
-        <v>1</v>
+        <v>203.5</v>
       </c>
       <c r="K18" t="n">
-        <v>163.7</v>
+        <v>1</v>
       </c>
       <c r="L18" t="n">
-        <v>1</v>
+        <v>192.2</v>
       </c>
       <c r="M18" t="n">
-        <v>163.7</v>
+        <v>0.6</v>
       </c>
       <c r="N18" t="n">
-        <v>1</v>
+        <v>192.2</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.6</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>a_09s.png</t>
-        </is>
+        <v>5</v>
+      </c>
+      <c r="B19" t="n">
+        <v>2</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -1399,44 +1420,45 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>214.7</v>
+        <v>202.5</v>
       </c>
       <c r="F19" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="G19" t="n">
-        <v>214.3</v>
+        <v>1</v>
       </c>
       <c r="H19" t="n">
-        <v>1</v>
+        <v>200.5</v>
       </c>
       <c r="I19" t="n">
-        <v>214.3</v>
+        <v>1</v>
       </c>
       <c r="J19" t="n">
-        <v>1</v>
+        <v>200.5</v>
       </c>
       <c r="K19" t="n">
-        <v>175.4</v>
+        <v>1</v>
       </c>
       <c r="L19" t="n">
-        <v>0.2</v>
+        <v>186.4</v>
       </c>
       <c r="M19" t="n">
-        <v>175.4</v>
+        <v>0.5</v>
       </c>
       <c r="N19" t="n">
-        <v>0.2</v>
+        <v>186.4</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>a_10k.png</t>
-        </is>
+        <v>9</v>
+      </c>
+      <c r="B20" t="n">
+        <v>3</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -1445,48 +1467,49 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Kam</t>
+          <t>Sm</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>164.8</v>
+        <v>207</v>
       </c>
       <c r="F20" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G20" t="n">
-        <v>164.8</v>
+        <v>1</v>
       </c>
       <c r="H20" t="n">
-        <v>1</v>
+        <v>206.9</v>
       </c>
       <c r="I20" t="n">
-        <v>164.8</v>
+        <v>1</v>
       </c>
       <c r="J20" t="n">
-        <v>1</v>
+        <v>206.9</v>
       </c>
       <c r="K20" t="n">
-        <v>164.8</v>
+        <v>1</v>
       </c>
       <c r="L20" t="n">
-        <v>1</v>
+        <v>194.9</v>
       </c>
       <c r="M20" t="n">
-        <v>164.8</v>
+        <v>0.5</v>
       </c>
       <c r="N20" t="n">
-        <v>1</v>
+        <v>194.9</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>a_10s.png</t>
-        </is>
+        <v>13</v>
+      </c>
+      <c r="B21" t="n">
+        <v>4</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1499,44 +1522,45 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>218.2</v>
+        <v>196.4</v>
       </c>
       <c r="F21" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G21" t="n">
-        <v>217.7</v>
+        <v>1</v>
       </c>
       <c r="H21" t="n">
-        <v>1</v>
+        <v>196.1</v>
       </c>
       <c r="I21" t="n">
-        <v>217.7</v>
+        <v>1</v>
       </c>
       <c r="J21" t="n">
-        <v>1</v>
+        <v>196.1</v>
       </c>
       <c r="K21" t="n">
-        <v>177.3</v>
+        <v>1</v>
       </c>
       <c r="L21" t="n">
-        <v>0.2</v>
+        <v>176.6</v>
       </c>
       <c r="M21" t="n">
-        <v>177.3</v>
+        <v>0.6</v>
       </c>
       <c r="N21" t="n">
-        <v>0.2</v>
+        <v>176.6</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0.6</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>a_11k.png</t>
-        </is>
+        <v>17</v>
+      </c>
+      <c r="B22" t="n">
+        <v>5</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1545,48 +1569,49 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Kam</t>
+          <t>Sm</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>163.1</v>
+        <v>208.3</v>
       </c>
       <c r="F22" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G22" t="n">
-        <v>163.1</v>
+        <v>1</v>
       </c>
       <c r="H22" t="n">
-        <v>1</v>
+        <v>208.1</v>
       </c>
       <c r="I22" t="n">
-        <v>163.1</v>
+        <v>1</v>
       </c>
       <c r="J22" t="n">
-        <v>1</v>
+        <v>208.1</v>
       </c>
       <c r="K22" t="n">
-        <v>163.1</v>
+        <v>1</v>
       </c>
       <c r="L22" t="n">
-        <v>1</v>
+        <v>190.9</v>
       </c>
       <c r="M22" t="n">
-        <v>163.1</v>
+        <v>0.4</v>
       </c>
       <c r="N22" t="n">
-        <v>1</v>
+        <v>190.9</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0.4</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>a_11s.png</t>
-        </is>
+      <c r="B23" t="n">
+        <v>6</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1599,44 +1624,45 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>215.6</v>
+        <v>211.3</v>
       </c>
       <c r="F23" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G23" t="n">
-        <v>215.2</v>
+        <v>1</v>
       </c>
       <c r="H23" t="n">
-        <v>1</v>
+        <v>211.1</v>
       </c>
       <c r="I23" t="n">
-        <v>215.2</v>
+        <v>1</v>
       </c>
       <c r="J23" t="n">
-        <v>1</v>
+        <v>211.1</v>
       </c>
       <c r="K23" t="n">
-        <v>158.1</v>
+        <v>1</v>
       </c>
       <c r="L23" t="n">
-        <v>0.2</v>
+        <v>182.1</v>
       </c>
       <c r="M23" t="n">
-        <v>158.1</v>
+        <v>0.3</v>
       </c>
       <c r="N23" t="n">
-        <v>0.2</v>
+        <v>182.1</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0.3</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>a_12k.png</t>
-        </is>
+        <v>25</v>
+      </c>
+      <c r="B24" t="n">
+        <v>7</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1645,48 +1671,49 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Kam</t>
+          <t>Sm</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>158.4</v>
+        <v>208.7</v>
       </c>
       <c r="F24" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G24" t="n">
-        <v>158</v>
+        <v>1</v>
       </c>
       <c r="H24" t="n">
-        <v>1</v>
+        <v>207.2</v>
       </c>
       <c r="I24" t="n">
-        <v>158</v>
+        <v>1</v>
       </c>
       <c r="J24" t="n">
-        <v>1</v>
+        <v>207.2</v>
       </c>
       <c r="K24" t="n">
-        <v>158.4</v>
+        <v>1</v>
       </c>
       <c r="L24" t="n">
-        <v>1</v>
+        <v>159.8</v>
       </c>
       <c r="M24" t="n">
-        <v>158.4</v>
+        <v>0.2</v>
       </c>
       <c r="N24" t="n">
-        <v>1</v>
+        <v>159.8</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>a_12s.png</t>
-        </is>
+        <v>29</v>
+      </c>
+      <c r="B25" t="n">
+        <v>8</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1699,44 +1726,45 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>209.9</v>
+        <v>213.5</v>
       </c>
       <c r="F25" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G25" t="n">
-        <v>208.2</v>
+        <v>1</v>
       </c>
       <c r="H25" t="n">
-        <v>1</v>
+        <v>213</v>
       </c>
       <c r="I25" t="n">
-        <v>208.2</v>
+        <v>1</v>
       </c>
       <c r="J25" t="n">
-        <v>1</v>
+        <v>213</v>
       </c>
       <c r="K25" t="n">
-        <v>151.4</v>
+        <v>1</v>
       </c>
       <c r="L25" t="n">
+        <v>159.8</v>
+      </c>
+      <c r="M25" t="n">
         <v>0.2</v>
       </c>
-      <c r="M25" t="n">
-        <v>151.4</v>
-      </c>
       <c r="N25" t="n">
+        <v>159.8</v>
+      </c>
+      <c r="O25" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>a_13k.png</t>
-        </is>
+        <v>33</v>
+      </c>
+      <c r="B26" t="n">
+        <v>9</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1745,48 +1773,49 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Kam</t>
+          <t>Sm</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>155.6</v>
+        <v>214.7</v>
       </c>
       <c r="F26" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G26" t="n">
-        <v>155.4</v>
+        <v>1</v>
       </c>
       <c r="H26" t="n">
-        <v>1</v>
+        <v>214.3</v>
       </c>
       <c r="I26" t="n">
-        <v>155.4</v>
+        <v>1</v>
       </c>
       <c r="J26" t="n">
-        <v>1</v>
+        <v>214.3</v>
       </c>
       <c r="K26" t="n">
-        <v>155.6</v>
+        <v>1</v>
       </c>
       <c r="L26" t="n">
-        <v>1</v>
+        <v>175.4</v>
       </c>
       <c r="M26" t="n">
-        <v>155.6</v>
+        <v>0.2</v>
       </c>
       <c r="N26" t="n">
-        <v>1</v>
+        <v>175.4</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>a_13s.png</t>
-        </is>
+        <v>37</v>
+      </c>
+      <c r="B27" t="n">
+        <v>10</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1799,44 +1828,45 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>205.5</v>
+        <v>218.2</v>
       </c>
       <c r="F27" t="n">
         <v>1</v>
       </c>
       <c r="G27" t="n">
-        <v>203.6</v>
+        <v>1</v>
       </c>
       <c r="H27" t="n">
-        <v>1</v>
+        <v>217.7</v>
       </c>
       <c r="I27" t="n">
-        <v>203.6</v>
+        <v>1</v>
       </c>
       <c r="J27" t="n">
-        <v>1</v>
+        <v>217.7</v>
       </c>
       <c r="K27" t="n">
-        <v>155.3</v>
+        <v>1</v>
       </c>
       <c r="L27" t="n">
-        <v>0.3</v>
+        <v>177.3</v>
       </c>
       <c r="M27" t="n">
-        <v>155.3</v>
+        <v>0.2</v>
       </c>
       <c r="N27" t="n">
-        <v>0.3</v>
+        <v>177.3</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>a_14k.png</t>
-        </is>
+        <v>41</v>
+      </c>
+      <c r="B28" t="n">
+        <v>11</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1845,48 +1875,49 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Kam</t>
+          <t>Sm</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>161.1</v>
+        <v>215.6</v>
       </c>
       <c r="F28" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G28" t="n">
-        <v>161.1</v>
+        <v>1</v>
       </c>
       <c r="H28" t="n">
-        <v>1</v>
+        <v>215.2</v>
       </c>
       <c r="I28" t="n">
-        <v>161.1</v>
+        <v>1</v>
       </c>
       <c r="J28" t="n">
-        <v>1</v>
+        <v>215.2</v>
       </c>
       <c r="K28" t="n">
-        <v>161.1</v>
+        <v>1</v>
       </c>
       <c r="L28" t="n">
-        <v>1</v>
+        <v>158.1</v>
       </c>
       <c r="M28" t="n">
-        <v>161.1</v>
+        <v>0.2</v>
       </c>
       <c r="N28" t="n">
-        <v>1</v>
+        <v>158.1</v>
+      </c>
+      <c r="O28" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>a_14s.png</t>
-        </is>
+        <v>45</v>
+      </c>
+      <c r="B29" t="n">
+        <v>12</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1899,44 +1930,45 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>210.9</v>
+        <v>209.9</v>
       </c>
       <c r="F29" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G29" t="n">
-        <v>210.3</v>
+        <v>1</v>
       </c>
       <c r="H29" t="n">
-        <v>1</v>
+        <v>208.2</v>
       </c>
       <c r="I29" t="n">
-        <v>210.3</v>
+        <v>1</v>
       </c>
       <c r="J29" t="n">
-        <v>1</v>
+        <v>208.2</v>
       </c>
       <c r="K29" t="n">
-        <v>170.6</v>
+        <v>1</v>
       </c>
       <c r="L29" t="n">
-        <v>0.3</v>
+        <v>151.4</v>
       </c>
       <c r="M29" t="n">
-        <v>170.6</v>
+        <v>0.2</v>
       </c>
       <c r="N29" t="n">
-        <v>0.3</v>
+        <v>151.4</v>
+      </c>
+      <c r="O29" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>a_15k.png</t>
-        </is>
+        <v>49</v>
+      </c>
+      <c r="B30" t="n">
+        <v>13</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1945,48 +1977,49 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Kam</t>
+          <t>Sm</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>163.7</v>
+        <v>205.5</v>
       </c>
       <c r="F30" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G30" t="n">
-        <v>161</v>
+        <v>1</v>
       </c>
       <c r="H30" t="n">
-        <v>1</v>
+        <v>203.6</v>
       </c>
       <c r="I30" t="n">
-        <v>161</v>
+        <v>1</v>
       </c>
       <c r="J30" t="n">
-        <v>1</v>
+        <v>203.6</v>
       </c>
       <c r="K30" t="n">
-        <v>163.7</v>
+        <v>1</v>
       </c>
       <c r="L30" t="n">
-        <v>1</v>
+        <v>155.3</v>
       </c>
       <c r="M30" t="n">
-        <v>163.7</v>
+        <v>0.3</v>
       </c>
       <c r="N30" t="n">
-        <v>1</v>
+        <v>155.3</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0.3</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>a_15s.png</t>
-        </is>
+        <v>53</v>
+      </c>
+      <c r="B31" t="n">
+        <v>14</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1999,44 +2032,45 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>217.6</v>
+        <v>210.9</v>
       </c>
       <c r="F31" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G31" t="n">
-        <v>214.9</v>
+        <v>1</v>
       </c>
       <c r="H31" t="n">
-        <v>1</v>
+        <v>210.3</v>
       </c>
       <c r="I31" t="n">
-        <v>214.9</v>
+        <v>1</v>
       </c>
       <c r="J31" t="n">
-        <v>1</v>
+        <v>210.3</v>
       </c>
       <c r="K31" t="n">
-        <v>159.6</v>
+        <v>1</v>
       </c>
       <c r="L31" t="n">
-        <v>0.2</v>
+        <v>170.6</v>
       </c>
       <c r="M31" t="n">
-        <v>159.6</v>
+        <v>0.3</v>
       </c>
       <c r="N31" t="n">
-        <v>0.2</v>
+        <v>170.6</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0.3</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>a_16k.png</t>
-        </is>
+        <v>57</v>
+      </c>
+      <c r="B32" t="n">
+        <v>15</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -2045,48 +2079,49 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Kam</t>
+          <t>Sm</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>158.2</v>
+        <v>217.6</v>
       </c>
       <c r="F32" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G32" t="n">
-        <v>157.9</v>
+        <v>1</v>
       </c>
       <c r="H32" t="n">
-        <v>1</v>
+        <v>214.9</v>
       </c>
       <c r="I32" t="n">
-        <v>157.9</v>
+        <v>1</v>
       </c>
       <c r="J32" t="n">
-        <v>1</v>
+        <v>214.9</v>
       </c>
       <c r="K32" t="n">
-        <v>158.2</v>
+        <v>1</v>
       </c>
       <c r="L32" t="n">
-        <v>1</v>
+        <v>159.6</v>
       </c>
       <c r="M32" t="n">
-        <v>158.2</v>
+        <v>0.2</v>
       </c>
       <c r="N32" t="n">
-        <v>1</v>
+        <v>159.6</v>
+      </c>
+      <c r="O32" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>a_16s.png</t>
-        </is>
+        <v>61</v>
+      </c>
+      <c r="B33" t="n">
+        <v>16</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -2102,41 +2137,42 @@
         <v>211.3</v>
       </c>
       <c r="F33" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G33" t="n">
+        <v>1</v>
+      </c>
+      <c r="H33" t="n">
         <v>209.9</v>
       </c>
-      <c r="H33" t="n">
-        <v>1</v>
-      </c>
       <c r="I33" t="n">
+        <v>1</v>
+      </c>
+      <c r="J33" t="n">
         <v>209.9</v>
       </c>
-      <c r="J33" t="n">
-        <v>1</v>
-      </c>
       <c r="K33" t="n">
+        <v>1</v>
+      </c>
+      <c r="L33" t="n">
         <v>168.3</v>
       </c>
-      <c r="L33" t="n">
+      <c r="M33" t="n">
         <v>0.2</v>
       </c>
-      <c r="M33" t="n">
+      <c r="N33" t="n">
         <v>168.3</v>
       </c>
-      <c r="N33" t="n">
+      <c r="O33" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>f01_k.png</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="B34" t="n">
+        <v>1</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -2152,41 +2188,42 @@
         <v>146</v>
       </c>
       <c r="F34" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G34" t="n">
+        <v>1</v>
+      </c>
+      <c r="H34" t="n">
         <v>146</v>
       </c>
-      <c r="H34" t="n">
-        <v>1</v>
-      </c>
       <c r="I34" t="n">
+        <v>1</v>
+      </c>
+      <c r="J34" t="n">
         <v>146</v>
       </c>
-      <c r="J34" t="n">
-        <v>1</v>
-      </c>
       <c r="K34" t="n">
+        <v>1</v>
+      </c>
+      <c r="L34" t="n">
         <v>146</v>
       </c>
-      <c r="L34" t="n">
-        <v>1</v>
-      </c>
       <c r="M34" t="n">
+        <v>1</v>
+      </c>
+      <c r="N34" t="n">
         <v>146</v>
       </c>
-      <c r="N34" t="n">
+      <c r="O34" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>f02_k.png</t>
-        </is>
+        <v>6</v>
+      </c>
+      <c r="B35" t="n">
+        <v>2</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -2202,41 +2239,42 @@
         <v>141.7</v>
       </c>
       <c r="F35" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="G35" t="n">
+        <v>1</v>
+      </c>
+      <c r="H35" t="n">
         <v>141.7</v>
       </c>
-      <c r="H35" t="n">
-        <v>1</v>
-      </c>
       <c r="I35" t="n">
+        <v>1</v>
+      </c>
+      <c r="J35" t="n">
         <v>141.7</v>
       </c>
-      <c r="J35" t="n">
-        <v>1</v>
-      </c>
       <c r="K35" t="n">
+        <v>1</v>
+      </c>
+      <c r="L35" t="n">
         <v>141.7</v>
       </c>
-      <c r="L35" t="n">
-        <v>1</v>
-      </c>
       <c r="M35" t="n">
+        <v>1</v>
+      </c>
+      <c r="N35" t="n">
         <v>141.7</v>
       </c>
-      <c r="N35" t="n">
+      <c r="O35" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>f03_k.png</t>
-        </is>
+        <v>10</v>
+      </c>
+      <c r="B36" t="n">
+        <v>3</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -2252,41 +2290,42 @@
         <v>146.2</v>
       </c>
       <c r="F36" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G36" t="n">
+        <v>1</v>
+      </c>
+      <c r="H36" t="n">
         <v>146.2</v>
       </c>
-      <c r="H36" t="n">
-        <v>1</v>
-      </c>
       <c r="I36" t="n">
+        <v>1</v>
+      </c>
+      <c r="J36" t="n">
         <v>146.2</v>
       </c>
-      <c r="J36" t="n">
-        <v>1</v>
-      </c>
       <c r="K36" t="n">
+        <v>1</v>
+      </c>
+      <c r="L36" t="n">
         <v>146.2</v>
       </c>
-      <c r="L36" t="n">
-        <v>1</v>
-      </c>
       <c r="M36" t="n">
+        <v>1</v>
+      </c>
+      <c r="N36" t="n">
         <v>146.2</v>
       </c>
-      <c r="N36" t="n">
+      <c r="O36" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>f04_k.png</t>
-        </is>
+        <v>14</v>
+      </c>
+      <c r="B37" t="n">
+        <v>4</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -2302,41 +2341,42 @@
         <v>139.8</v>
       </c>
       <c r="F37" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G37" t="n">
+        <v>1</v>
+      </c>
+      <c r="H37" t="n">
         <v>139.8</v>
       </c>
-      <c r="H37" t="n">
-        <v>1</v>
-      </c>
       <c r="I37" t="n">
+        <v>1</v>
+      </c>
+      <c r="J37" t="n">
         <v>139.8</v>
       </c>
-      <c r="J37" t="n">
-        <v>1</v>
-      </c>
       <c r="K37" t="n">
+        <v>1</v>
+      </c>
+      <c r="L37" t="n">
         <v>139.8</v>
       </c>
-      <c r="L37" t="n">
-        <v>1</v>
-      </c>
       <c r="M37" t="n">
+        <v>1</v>
+      </c>
+      <c r="N37" t="n">
         <v>139.8</v>
       </c>
-      <c r="N37" t="n">
+      <c r="O37" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>f05_k.png</t>
-        </is>
+        <v>18</v>
+      </c>
+      <c r="B38" t="n">
+        <v>5</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -2352,41 +2392,42 @@
         <v>145.1</v>
       </c>
       <c r="F38" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G38" t="n">
+        <v>1</v>
+      </c>
+      <c r="H38" t="n">
         <v>145.1</v>
       </c>
-      <c r="H38" t="n">
-        <v>1</v>
-      </c>
       <c r="I38" t="n">
+        <v>1</v>
+      </c>
+      <c r="J38" t="n">
         <v>145.1</v>
       </c>
-      <c r="J38" t="n">
-        <v>1</v>
-      </c>
       <c r="K38" t="n">
+        <v>1</v>
+      </c>
+      <c r="L38" t="n">
         <v>145.1</v>
       </c>
-      <c r="L38" t="n">
-        <v>1</v>
-      </c>
       <c r="M38" t="n">
+        <v>1</v>
+      </c>
+      <c r="N38" t="n">
         <v>145.1</v>
       </c>
-      <c r="N38" t="n">
+      <c r="O38" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>f06_k.png</t>
-        </is>
+        <v>22</v>
+      </c>
+      <c r="B39" t="n">
+        <v>6</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -2402,41 +2443,42 @@
         <v>155</v>
       </c>
       <c r="F39" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G39" t="n">
+        <v>1</v>
+      </c>
+      <c r="H39" t="n">
         <v>155</v>
       </c>
-      <c r="H39" t="n">
-        <v>1</v>
-      </c>
       <c r="I39" t="n">
+        <v>1</v>
+      </c>
+      <c r="J39" t="n">
         <v>155</v>
       </c>
-      <c r="J39" t="n">
-        <v>1</v>
-      </c>
       <c r="K39" t="n">
+        <v>1</v>
+      </c>
+      <c r="L39" t="n">
         <v>155</v>
       </c>
-      <c r="L39" t="n">
-        <v>1</v>
-      </c>
       <c r="M39" t="n">
+        <v>1</v>
+      </c>
+      <c r="N39" t="n">
         <v>155</v>
       </c>
-      <c r="N39" t="n">
+      <c r="O39" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>38</v>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>f07_k.png</t>
-        </is>
+        <v>26</v>
+      </c>
+      <c r="B40" t="n">
+        <v>7</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -2452,41 +2494,42 @@
         <v>155</v>
       </c>
       <c r="F40" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G40" t="n">
+        <v>1</v>
+      </c>
+      <c r="H40" t="n">
         <v>155</v>
       </c>
-      <c r="H40" t="n">
-        <v>1</v>
-      </c>
       <c r="I40" t="n">
+        <v>1</v>
+      </c>
+      <c r="J40" t="n">
         <v>155</v>
       </c>
-      <c r="J40" t="n">
-        <v>1</v>
-      </c>
       <c r="K40" t="n">
+        <v>1</v>
+      </c>
+      <c r="L40" t="n">
         <v>155</v>
       </c>
-      <c r="L40" t="n">
-        <v>1</v>
-      </c>
       <c r="M40" t="n">
+        <v>1</v>
+      </c>
+      <c r="N40" t="n">
         <v>155</v>
       </c>
-      <c r="N40" t="n">
+      <c r="O40" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>f08_k.png</t>
-        </is>
+        <v>30</v>
+      </c>
+      <c r="B41" t="n">
+        <v>8</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -2502,41 +2545,42 @@
         <v>154.4</v>
       </c>
       <c r="F41" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G41" t="n">
+        <v>1</v>
+      </c>
+      <c r="H41" t="n">
         <v>154.4</v>
       </c>
-      <c r="H41" t="n">
-        <v>1</v>
-      </c>
       <c r="I41" t="n">
+        <v>1</v>
+      </c>
+      <c r="J41" t="n">
         <v>154.4</v>
       </c>
-      <c r="J41" t="n">
-        <v>1</v>
-      </c>
       <c r="K41" t="n">
+        <v>1</v>
+      </c>
+      <c r="L41" t="n">
         <v>154.4</v>
       </c>
-      <c r="L41" t="n">
-        <v>1</v>
-      </c>
       <c r="M41" t="n">
+        <v>1</v>
+      </c>
+      <c r="N41" t="n">
         <v>154.4</v>
       </c>
-      <c r="N41" t="n">
+      <c r="O41" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>f09_k.png</t>
-        </is>
+        <v>34</v>
+      </c>
+      <c r="B42" t="n">
+        <v>9</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -2552,41 +2596,42 @@
         <v>155.8</v>
       </c>
       <c r="F42" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G42" t="n">
+        <v>1</v>
+      </c>
+      <c r="H42" t="n">
         <v>155.8</v>
       </c>
-      <c r="H42" t="n">
-        <v>1</v>
-      </c>
       <c r="I42" t="n">
+        <v>1</v>
+      </c>
+      <c r="J42" t="n">
         <v>155.8</v>
       </c>
-      <c r="J42" t="n">
-        <v>1</v>
-      </c>
       <c r="K42" t="n">
+        <v>1</v>
+      </c>
+      <c r="L42" t="n">
         <v>155.8</v>
       </c>
-      <c r="L42" t="n">
-        <v>1</v>
-      </c>
       <c r="M42" t="n">
+        <v>1</v>
+      </c>
+      <c r="N42" t="n">
         <v>155.8</v>
       </c>
-      <c r="N42" t="n">
+      <c r="O42" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>f10_k.png</t>
-        </is>
+        <v>38</v>
+      </c>
+      <c r="B43" t="n">
+        <v>10</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -2602,30 +2647,33 @@
         <v>154.8</v>
       </c>
       <c r="F43" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G43" t="n">
+        <v>1</v>
+      </c>
+      <c r="H43" t="n">
         <v>154.8</v>
       </c>
-      <c r="H43" t="n">
-        <v>1</v>
-      </c>
       <c r="I43" t="n">
+        <v>1</v>
+      </c>
+      <c r="J43" t="n">
         <v>154.8</v>
       </c>
-      <c r="J43" t="n">
-        <v>1</v>
-      </c>
       <c r="K43" t="n">
+        <v>1</v>
+      </c>
+      <c r="L43" t="n">
         <v>154.8</v>
       </c>
-      <c r="L43" t="n">
-        <v>1</v>
-      </c>
       <c r="M43" t="n">
+        <v>1</v>
+      </c>
+      <c r="N43" t="n">
         <v>154.8</v>
       </c>
-      <c r="N43" t="n">
+      <c r="O43" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2633,10 +2681,8 @@
       <c r="A44" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>f11_k.png</t>
-        </is>
+      <c r="B44" t="n">
+        <v>11</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -2652,41 +2698,42 @@
         <v>157.5</v>
       </c>
       <c r="F44" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G44" t="n">
+        <v>1</v>
+      </c>
+      <c r="H44" t="n">
         <v>157.5</v>
       </c>
-      <c r="H44" t="n">
-        <v>1</v>
-      </c>
       <c r="I44" t="n">
+        <v>1</v>
+      </c>
+      <c r="J44" t="n">
         <v>157.5</v>
       </c>
-      <c r="J44" t="n">
-        <v>1</v>
-      </c>
       <c r="K44" t="n">
+        <v>1</v>
+      </c>
+      <c r="L44" t="n">
         <v>157.5</v>
       </c>
-      <c r="L44" t="n">
-        <v>1</v>
-      </c>
       <c r="M44" t="n">
+        <v>1</v>
+      </c>
+      <c r="N44" t="n">
         <v>157.5</v>
       </c>
-      <c r="N44" t="n">
+      <c r="O44" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>f12_k.png</t>
-        </is>
+        <v>46</v>
+      </c>
+      <c r="B45" t="n">
+        <v>12</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -2705,38 +2752,39 @@
         <v>1</v>
       </c>
       <c r="G45" t="n">
+        <v>1</v>
+      </c>
+      <c r="H45" t="n">
         <v>157.8</v>
       </c>
-      <c r="H45" t="n">
-        <v>1</v>
-      </c>
       <c r="I45" t="n">
+        <v>1</v>
+      </c>
+      <c r="J45" t="n">
         <v>157.8</v>
       </c>
-      <c r="J45" t="n">
-        <v>1</v>
-      </c>
       <c r="K45" t="n">
+        <v>1</v>
+      </c>
+      <c r="L45" t="n">
         <v>157.8</v>
       </c>
-      <c r="L45" t="n">
-        <v>1</v>
-      </c>
       <c r="M45" t="n">
+        <v>1</v>
+      </c>
+      <c r="N45" t="n">
         <v>157.8</v>
       </c>
-      <c r="N45" t="n">
+      <c r="O45" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>f13_k.png</t>
-        </is>
+        <v>50</v>
+      </c>
+      <c r="B46" t="n">
+        <v>13</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -2752,41 +2800,42 @@
         <v>155.3</v>
       </c>
       <c r="F46" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G46" t="n">
+        <v>1</v>
+      </c>
+      <c r="H46" t="n">
         <v>155.3</v>
       </c>
-      <c r="H46" t="n">
-        <v>1</v>
-      </c>
       <c r="I46" t="n">
+        <v>1</v>
+      </c>
+      <c r="J46" t="n">
         <v>155.3</v>
       </c>
-      <c r="J46" t="n">
-        <v>1</v>
-      </c>
       <c r="K46" t="n">
+        <v>1</v>
+      </c>
+      <c r="L46" t="n">
         <v>155.3</v>
       </c>
-      <c r="L46" t="n">
-        <v>1</v>
-      </c>
       <c r="M46" t="n">
+        <v>1</v>
+      </c>
+      <c r="N46" t="n">
         <v>155.3</v>
       </c>
-      <c r="N46" t="n">
+      <c r="O46" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>f14_k.png</t>
-        </is>
+        <v>54</v>
+      </c>
+      <c r="B47" t="n">
+        <v>14</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -2802,41 +2851,42 @@
         <v>157.7</v>
       </c>
       <c r="F47" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G47" t="n">
+        <v>1</v>
+      </c>
+      <c r="H47" t="n">
         <v>157.7</v>
       </c>
-      <c r="H47" t="n">
-        <v>1</v>
-      </c>
       <c r="I47" t="n">
+        <v>1</v>
+      </c>
+      <c r="J47" t="n">
         <v>157.7</v>
       </c>
-      <c r="J47" t="n">
-        <v>1</v>
-      </c>
       <c r="K47" t="n">
+        <v>1</v>
+      </c>
+      <c r="L47" t="n">
         <v>157.7</v>
       </c>
-      <c r="L47" t="n">
-        <v>1</v>
-      </c>
       <c r="M47" t="n">
+        <v>1</v>
+      </c>
+      <c r="N47" t="n">
         <v>157.7</v>
       </c>
-      <c r="N47" t="n">
+      <c r="O47" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>f15_k.png</t>
-        </is>
+        <v>58</v>
+      </c>
+      <c r="B48" t="n">
+        <v>15</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -2852,41 +2902,42 @@
         <v>151.1</v>
       </c>
       <c r="F48" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G48" t="n">
+        <v>1</v>
+      </c>
+      <c r="H48" t="n">
         <v>148.8</v>
       </c>
-      <c r="H48" t="n">
-        <v>1</v>
-      </c>
       <c r="I48" t="n">
+        <v>1</v>
+      </c>
+      <c r="J48" t="n">
         <v>148.8</v>
       </c>
-      <c r="J48" t="n">
-        <v>1</v>
-      </c>
       <c r="K48" t="n">
+        <v>1</v>
+      </c>
+      <c r="L48" t="n">
         <v>151.1</v>
       </c>
-      <c r="L48" t="n">
-        <v>1</v>
-      </c>
       <c r="M48" t="n">
+        <v>1</v>
+      </c>
+      <c r="N48" t="n">
         <v>151.1</v>
       </c>
-      <c r="N48" t="n">
+      <c r="O48" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>47</v>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>f16_k.png</t>
-        </is>
+        <v>62</v>
+      </c>
+      <c r="B49" t="n">
+        <v>16</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -2902,41 +2953,42 @@
         <v>147.3</v>
       </c>
       <c r="F49" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G49" t="n">
+        <v>1</v>
+      </c>
+      <c r="H49" t="n">
         <v>147.2</v>
       </c>
-      <c r="H49" t="n">
-        <v>1</v>
-      </c>
       <c r="I49" t="n">
+        <v>1</v>
+      </c>
+      <c r="J49" t="n">
         <v>147.2</v>
       </c>
-      <c r="J49" t="n">
-        <v>1</v>
-      </c>
       <c r="K49" t="n">
+        <v>1</v>
+      </c>
+      <c r="L49" t="n">
         <v>147.3</v>
       </c>
-      <c r="L49" t="n">
-        <v>1</v>
-      </c>
       <c r="M49" t="n">
+        <v>1</v>
+      </c>
+      <c r="N49" t="n">
         <v>147.3</v>
       </c>
-      <c r="N49" t="n">
+      <c r="O49" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>f_01s.png</t>
-        </is>
+        <v>3</v>
+      </c>
+      <c r="B50" t="n">
+        <v>1</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -2952,41 +3004,42 @@
         <v>212.8</v>
       </c>
       <c r="F50" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G50" t="n">
+        <v>1</v>
+      </c>
+      <c r="H50" t="n">
         <v>212.7</v>
       </c>
-      <c r="H50" t="n">
-        <v>1</v>
-      </c>
       <c r="I50" t="n">
+        <v>1</v>
+      </c>
+      <c r="J50" t="n">
         <v>212.7</v>
       </c>
-      <c r="J50" t="n">
-        <v>1</v>
-      </c>
       <c r="K50" t="n">
+        <v>1</v>
+      </c>
+      <c r="L50" t="n">
         <v>179.9</v>
       </c>
-      <c r="L50" t="n">
+      <c r="M50" t="n">
         <v>0.2</v>
       </c>
-      <c r="M50" t="n">
+      <c r="N50" t="n">
         <v>179.9</v>
       </c>
-      <c r="N50" t="n">
+      <c r="O50" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>f_02s.png</t>
-        </is>
+        <v>7</v>
+      </c>
+      <c r="B51" t="n">
+        <v>2</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -3002,41 +3055,42 @@
         <v>207.1</v>
       </c>
       <c r="F51" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G51" t="n">
+        <v>1</v>
+      </c>
+      <c r="H51" t="n">
         <v>206.6</v>
       </c>
-      <c r="H51" t="n">
-        <v>1</v>
-      </c>
       <c r="I51" t="n">
+        <v>1</v>
+      </c>
+      <c r="J51" t="n">
         <v>206.6</v>
       </c>
-      <c r="J51" t="n">
-        <v>1</v>
-      </c>
       <c r="K51" t="n">
+        <v>1</v>
+      </c>
+      <c r="L51" t="n">
         <v>169.7</v>
       </c>
-      <c r="L51" t="n">
+      <c r="M51" t="n">
         <v>0.3</v>
       </c>
-      <c r="M51" t="n">
+      <c r="N51" t="n">
         <v>169.7</v>
       </c>
-      <c r="N51" t="n">
+      <c r="O51" t="n">
         <v>0.3</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>f_03s.png</t>
-        </is>
+        <v>11</v>
+      </c>
+      <c r="B52" t="n">
+        <v>3</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -3052,41 +3106,42 @@
         <v>209.5</v>
       </c>
       <c r="F52" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G52" t="n">
+        <v>1</v>
+      </c>
+      <c r="H52" t="n">
         <v>209</v>
       </c>
-      <c r="H52" t="n">
-        <v>1</v>
-      </c>
       <c r="I52" t="n">
+        <v>1</v>
+      </c>
+      <c r="J52" t="n">
         <v>209</v>
       </c>
-      <c r="J52" t="n">
-        <v>1</v>
-      </c>
       <c r="K52" t="n">
+        <v>1</v>
+      </c>
+      <c r="L52" t="n">
         <v>190</v>
       </c>
-      <c r="L52" t="n">
+      <c r="M52" t="n">
         <v>0.4</v>
       </c>
-      <c r="M52" t="n">
+      <c r="N52" t="n">
         <v>190</v>
       </c>
-      <c r="N52" t="n">
+      <c r="O52" t="n">
         <v>0.4</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>51</v>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>f_04s.png</t>
-        </is>
+        <v>15</v>
+      </c>
+      <c r="B53" t="n">
+        <v>4</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -3102,41 +3157,42 @@
         <v>197.4</v>
       </c>
       <c r="F53" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G53" t="n">
+        <v>1</v>
+      </c>
+      <c r="H53" t="n">
         <v>196.1</v>
       </c>
-      <c r="H53" t="n">
-        <v>1</v>
-      </c>
       <c r="I53" t="n">
+        <v>1</v>
+      </c>
+      <c r="J53" t="n">
         <v>196.1</v>
       </c>
-      <c r="J53" t="n">
-        <v>1</v>
-      </c>
       <c r="K53" t="n">
+        <v>1</v>
+      </c>
+      <c r="L53" t="n">
         <v>184.5</v>
       </c>
-      <c r="L53" t="n">
+      <c r="M53" t="n">
         <v>0.6</v>
       </c>
-      <c r="M53" t="n">
+      <c r="N53" t="n">
         <v>184.5</v>
       </c>
-      <c r="N53" t="n">
+      <c r="O53" t="n">
         <v>0.6</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>52</v>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>f_05s.png</t>
-        </is>
+        <v>19</v>
+      </c>
+      <c r="B54" t="n">
+        <v>5</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -3152,41 +3208,42 @@
         <v>202.8</v>
       </c>
       <c r="F54" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G54" t="n">
+        <v>1</v>
+      </c>
+      <c r="H54" t="n">
         <v>202.6</v>
       </c>
-      <c r="H54" t="n">
-        <v>1</v>
-      </c>
       <c r="I54" t="n">
+        <v>1</v>
+      </c>
+      <c r="J54" t="n">
         <v>202.6</v>
       </c>
-      <c r="J54" t="n">
-        <v>1</v>
-      </c>
       <c r="K54" t="n">
+        <v>1</v>
+      </c>
+      <c r="L54" t="n">
         <v>199.1</v>
       </c>
-      <c r="L54" t="n">
+      <c r="M54" t="n">
         <v>0.8</v>
       </c>
-      <c r="M54" t="n">
+      <c r="N54" t="n">
         <v>199.1</v>
       </c>
-      <c r="N54" t="n">
+      <c r="O54" t="n">
         <v>0.8</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>53</v>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>f_06s.png</t>
-        </is>
+        <v>23</v>
+      </c>
+      <c r="B55" t="n">
+        <v>6</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -3202,41 +3259,42 @@
         <v>212.6</v>
       </c>
       <c r="F55" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G55" t="n">
+        <v>1</v>
+      </c>
+      <c r="H55" t="n">
         <v>211.8</v>
       </c>
-      <c r="H55" t="n">
-        <v>1</v>
-      </c>
       <c r="I55" t="n">
+        <v>1</v>
+      </c>
+      <c r="J55" t="n">
         <v>211.8</v>
       </c>
-      <c r="J55" t="n">
-        <v>1</v>
-      </c>
       <c r="K55" t="n">
+        <v>1</v>
+      </c>
+      <c r="L55" t="n">
         <v>179.9</v>
       </c>
-      <c r="L55" t="n">
+      <c r="M55" t="n">
         <v>0.2</v>
       </c>
-      <c r="M55" t="n">
+      <c r="N55" t="n">
         <v>179.9</v>
       </c>
-      <c r="N55" t="n">
+      <c r="O55" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>54</v>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>f_07s.png</t>
-        </is>
+        <v>27</v>
+      </c>
+      <c r="B56" t="n">
+        <v>7</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -3252,41 +3310,42 @@
         <v>215.5</v>
       </c>
       <c r="F56" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G56" t="n">
+        <v>1</v>
+      </c>
+      <c r="H56" t="n">
         <v>214.6</v>
       </c>
-      <c r="H56" t="n">
-        <v>1</v>
-      </c>
       <c r="I56" t="n">
+        <v>1</v>
+      </c>
+      <c r="J56" t="n">
         <v>214.6</v>
       </c>
-      <c r="J56" t="n">
-        <v>1</v>
-      </c>
       <c r="K56" t="n">
+        <v>1</v>
+      </c>
+      <c r="L56" t="n">
         <v>169.5</v>
       </c>
-      <c r="L56" t="n">
+      <c r="M56" t="n">
         <v>0.2</v>
       </c>
-      <c r="M56" t="n">
+      <c r="N56" t="n">
         <v>169.5</v>
       </c>
-      <c r="N56" t="n">
+      <c r="O56" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>f_08s.png</t>
-        </is>
+        <v>31</v>
+      </c>
+      <c r="B57" t="n">
+        <v>8</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -3302,41 +3361,42 @@
         <v>215.2</v>
       </c>
       <c r="F57" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G57" t="n">
+        <v>1</v>
+      </c>
+      <c r="H57" t="n">
         <v>214.5</v>
       </c>
-      <c r="H57" t="n">
-        <v>1</v>
-      </c>
       <c r="I57" t="n">
+        <v>1</v>
+      </c>
+      <c r="J57" t="n">
         <v>214.5</v>
       </c>
-      <c r="J57" t="n">
-        <v>1</v>
-      </c>
       <c r="K57" t="n">
+        <v>1</v>
+      </c>
+      <c r="L57" t="n">
         <v>171.9</v>
       </c>
-      <c r="L57" t="n">
+      <c r="M57" t="n">
         <v>0.2</v>
       </c>
-      <c r="M57" t="n">
+      <c r="N57" t="n">
         <v>171.9</v>
       </c>
-      <c r="N57" t="n">
+      <c r="O57" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>f_09s.png</t>
-        </is>
+        <v>35</v>
+      </c>
+      <c r="B58" t="n">
+        <v>9</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -3352,41 +3412,42 @@
         <v>210.1</v>
       </c>
       <c r="F58" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G58" t="n">
+        <v>1</v>
+      </c>
+      <c r="H58" t="n">
         <v>209.2</v>
       </c>
-      <c r="H58" t="n">
-        <v>1</v>
-      </c>
       <c r="I58" t="n">
+        <v>1</v>
+      </c>
+      <c r="J58" t="n">
         <v>209.2</v>
       </c>
-      <c r="J58" t="n">
-        <v>1</v>
-      </c>
       <c r="K58" t="n">
+        <v>1</v>
+      </c>
+      <c r="L58" t="n">
         <v>196.3</v>
       </c>
-      <c r="L58" t="n">
+      <c r="M58" t="n">
         <v>0.5</v>
       </c>
-      <c r="M58" t="n">
+      <c r="N58" t="n">
         <v>196.3</v>
       </c>
-      <c r="N58" t="n">
+      <c r="O58" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>57</v>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>f_10s.png</t>
-        </is>
+        <v>39</v>
+      </c>
+      <c r="B59" t="n">
+        <v>10</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -3402,41 +3463,42 @@
         <v>203.6</v>
       </c>
       <c r="F59" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G59" t="n">
+        <v>1</v>
+      </c>
+      <c r="H59" t="n">
         <v>203.4</v>
       </c>
-      <c r="H59" t="n">
-        <v>1</v>
-      </c>
       <c r="I59" t="n">
+        <v>1</v>
+      </c>
+      <c r="J59" t="n">
         <v>203.4</v>
       </c>
-      <c r="J59" t="n">
-        <v>1</v>
-      </c>
       <c r="K59" t="n">
+        <v>1</v>
+      </c>
+      <c r="L59" t="n">
         <v>200.4</v>
       </c>
-      <c r="L59" t="n">
+      <c r="M59" t="n">
         <v>0.8</v>
       </c>
-      <c r="M59" t="n">
+      <c r="N59" t="n">
         <v>200.4</v>
       </c>
-      <c r="N59" t="n">
+      <c r="O59" t="n">
         <v>0.8</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>58</v>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>f_11s.png</t>
-        </is>
+        <v>43</v>
+      </c>
+      <c r="B60" t="n">
+        <v>11</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -3452,41 +3514,42 @@
         <v>212.1</v>
       </c>
       <c r="F60" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G60" t="n">
+        <v>1</v>
+      </c>
+      <c r="H60" t="n">
         <v>211.9</v>
       </c>
-      <c r="H60" t="n">
-        <v>1</v>
-      </c>
       <c r="I60" t="n">
+        <v>1</v>
+      </c>
+      <c r="J60" t="n">
         <v>211.9</v>
       </c>
-      <c r="J60" t="n">
-        <v>1</v>
-      </c>
       <c r="K60" t="n">
+        <v>1</v>
+      </c>
+      <c r="L60" t="n">
         <v>163.2</v>
       </c>
-      <c r="L60" t="n">
+      <c r="M60" t="n">
         <v>0.2</v>
       </c>
-      <c r="M60" t="n">
+      <c r="N60" t="n">
         <v>163.2</v>
       </c>
-      <c r="N60" t="n">
+      <c r="O60" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>59</v>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>f_12s.png</t>
-        </is>
+        <v>47</v>
+      </c>
+      <c r="B61" t="n">
+        <v>12</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -3502,41 +3565,42 @@
         <v>215.8</v>
       </c>
       <c r="F61" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G61" t="n">
+        <v>1</v>
+      </c>
+      <c r="H61" t="n">
         <v>215.3</v>
       </c>
-      <c r="H61" t="n">
-        <v>1</v>
-      </c>
       <c r="I61" t="n">
+        <v>1</v>
+      </c>
+      <c r="J61" t="n">
         <v>215.3</v>
       </c>
-      <c r="J61" t="n">
-        <v>1</v>
-      </c>
       <c r="K61" t="n">
+        <v>1</v>
+      </c>
+      <c r="L61" t="n">
         <v>187.4</v>
       </c>
-      <c r="L61" t="n">
+      <c r="M61" t="n">
         <v>0.2</v>
       </c>
-      <c r="M61" t="n">
+      <c r="N61" t="n">
         <v>187.4</v>
       </c>
-      <c r="N61" t="n">
+      <c r="O61" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>f_13s.png</t>
-        </is>
+        <v>51</v>
+      </c>
+      <c r="B62" t="n">
+        <v>13</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -3555,38 +3619,39 @@
         <v>1</v>
       </c>
       <c r="G62" t="n">
+        <v>1</v>
+      </c>
+      <c r="H62" t="n">
         <v>216.9</v>
       </c>
-      <c r="H62" t="n">
-        <v>1</v>
-      </c>
       <c r="I62" t="n">
+        <v>1</v>
+      </c>
+      <c r="J62" t="n">
         <v>216.9</v>
       </c>
-      <c r="J62" t="n">
-        <v>1</v>
-      </c>
       <c r="K62" t="n">
+        <v>1</v>
+      </c>
+      <c r="L62" t="n">
         <v>168.7</v>
       </c>
-      <c r="L62" t="n">
+      <c r="M62" t="n">
         <v>0.2</v>
       </c>
-      <c r="M62" t="n">
+      <c r="N62" t="n">
         <v>168.7</v>
       </c>
-      <c r="N62" t="n">
+      <c r="O62" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>61</v>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>f_14s.png</t>
-        </is>
+        <v>55</v>
+      </c>
+      <c r="B63" t="n">
+        <v>14</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -3602,41 +3667,42 @@
         <v>216.1</v>
       </c>
       <c r="F63" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G63" t="n">
+        <v>1</v>
+      </c>
+      <c r="H63" t="n">
         <v>215.5</v>
       </c>
-      <c r="H63" t="n">
-        <v>1</v>
-      </c>
       <c r="I63" t="n">
+        <v>1</v>
+      </c>
+      <c r="J63" t="n">
         <v>215.5</v>
       </c>
-      <c r="J63" t="n">
-        <v>1</v>
-      </c>
       <c r="K63" t="n">
+        <v>1</v>
+      </c>
+      <c r="L63" t="n">
         <v>198.2</v>
       </c>
-      <c r="L63" t="n">
+      <c r="M63" t="n">
         <v>0.3</v>
       </c>
-      <c r="M63" t="n">
+      <c r="N63" t="n">
         <v>198.2</v>
       </c>
-      <c r="N63" t="n">
+      <c r="O63" t="n">
         <v>0.3</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>62</v>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>f_15s.png</t>
-        </is>
+        <v>59</v>
+      </c>
+      <c r="B64" t="n">
+        <v>15</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -3652,30 +3718,33 @@
         <v>203.3</v>
       </c>
       <c r="F64" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="G64" t="n">
+        <v>1</v>
+      </c>
+      <c r="H64" t="n">
         <v>199.6</v>
       </c>
-      <c r="H64" t="n">
-        <v>1</v>
-      </c>
       <c r="I64" t="n">
+        <v>1</v>
+      </c>
+      <c r="J64" t="n">
         <v>199.6</v>
       </c>
-      <c r="J64" t="n">
-        <v>1</v>
-      </c>
       <c r="K64" t="n">
+        <v>1</v>
+      </c>
+      <c r="L64" t="n">
         <v>197</v>
       </c>
-      <c r="L64" t="n">
+      <c r="M64" t="n">
         <v>0.7</v>
       </c>
-      <c r="M64" t="n">
+      <c r="N64" t="n">
         <v>197</v>
       </c>
-      <c r="N64" t="n">
+      <c r="O64" t="n">
         <v>0.7</v>
       </c>
     </row>
@@ -3683,10 +3752,8 @@
       <c r="A65" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>f_16s.png</t>
-        </is>
+      <c r="B65" t="n">
+        <v>16</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -3702,30 +3769,33 @@
         <v>206.6</v>
       </c>
       <c r="F65" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G65" t="n">
+        <v>1</v>
+      </c>
+      <c r="H65" t="n">
         <v>205.6</v>
       </c>
-      <c r="H65" t="n">
-        <v>1</v>
-      </c>
       <c r="I65" t="n">
+        <v>1</v>
+      </c>
+      <c r="J65" t="n">
         <v>205.6</v>
       </c>
-      <c r="J65" t="n">
-        <v>1</v>
-      </c>
       <c r="K65" t="n">
+        <v>1</v>
+      </c>
+      <c r="L65" t="n">
         <v>151.2</v>
       </c>
-      <c r="L65" t="n">
+      <c r="M65" t="n">
         <v>0.2</v>
       </c>
-      <c r="M65" t="n">
+      <c r="N65" t="n">
         <v>151.2</v>
       </c>
-      <c r="N65" t="n">
+      <c r="O65" t="n">
         <v>0.2</v>
       </c>
     </row>

</xml_diff>